<commit_message>
added incorrect answer messages
</commit_message>
<xml_diff>
--- a/scripts/CNC_Machining_Questions_0215.xlsx
+++ b/scripts/CNC_Machining_Questions_0215.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\risa.hirsh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5D5045-5C57-4817-BF91-95671B198D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C72A01A-35D3-4BE6-8BEB-4982A5E5E93E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3390" yWindow="3630" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11152,8 +11152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1269" workbookViewId="0">
-      <selection activeCell="C1275" sqref="C1275"/>
+    <sheetView tabSelected="1" topLeftCell="A408" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11890,7 +11890,7 @@
         <v>23</v>
       </c>
       <c r="D32" t="s">
-        <v>2789</v>
+        <v>2790</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>74</v>

</xml_diff>